<commit_message>
next set of revisions to paper + new plotting
</commit_message>
<xml_diff>
--- a/docs/paper/sample_expedition/CoordinatesExport-sample.xlsx
+++ b/docs/paper/sample_expedition/CoordinatesExport-sample.xlsx
@@ -582,7 +582,7 @@
         <x:v>-30.007831</x:v>
       </x:c>
       <x:c r="D2" s="5" t="n">
-        <x:v>31.456983</x:v>
+        <x:v>32.094662</x:v>
       </x:c>
       <x:c r="F2" s="1"/>
       <x:c r="G2" s="1"/>
@@ -606,10 +606,10 @@
         </x:is>
       </x:c>
       <x:c r="C3" s="6" t="n">
-        <x:v>-30.006505</x:v>
+        <x:v>-31.638883</x:v>
       </x:c>
       <x:c r="D3" s="5" t="n">
-        <x:v>31.814182</x:v>
+        <x:v>30.870622</x:v>
       </x:c>
       <x:c r="F3" s="1"/>
       <x:c r="G3" s="1"/>
@@ -633,10 +633,10 @@
         </x:is>
       </x:c>
       <x:c r="C4" s="6" t="n">
-        <x:v>-29.996594</x:v>
+        <x:v>-33.318683</x:v>
       </x:c>
       <x:c r="D4" s="5" t="n">
-        <x:v>32.150686</x:v>
+        <x:v>29.505758</x:v>
       </x:c>
       <x:c r="F4" s="1"/>
       <x:c r="G4" s="1"/>
@@ -660,10 +660,10 @@
         </x:is>
       </x:c>
       <x:c r="C5" s="6" t="n">
-        <x:v>-29.994966</x:v>
+        <x:v>-34.895537</x:v>
       </x:c>
       <x:c r="D5" s="5" t="n">
-        <x:v>32.522907</x:v>
+        <x:v>27.046444</x:v>
       </x:c>
       <x:c r="F5" s="1"/>
       <x:c r="G5" s="1"/>
@@ -687,10 +687,10 @@
         </x:is>
       </x:c>
       <x:c r="C6" s="6" t="n">
-        <x:v>-30.000326</x:v>
+        <x:v>-35.940604</x:v>
       </x:c>
       <x:c r="D6" s="5" t="n">
-        <x:v>32.843637</x:v>
+        <x:v>23.644859</x:v>
       </x:c>
       <x:c r="F6" s="1"/>
       <x:c r="G6" s="1"/>
@@ -714,10 +714,10 @@
         </x:is>
       </x:c>
       <x:c r="C7" s="6" t="n">
-        <x:v>-31.798692</x:v>
+        <x:v>-36.169229</x:v>
       </x:c>
       <x:c r="D7" s="5" t="n">
-        <x:v>30.949775</x:v>
+        <x:v>19.822039</x:v>
       </x:c>
       <x:c r="F7" s="1"/>
       <x:c r="G7" s="1"/>
@@ -741,10 +741,10 @@
         </x:is>
       </x:c>
       <x:c r="C8" s="6" t="n">
-        <x:v>-33.023785</x:v>
+        <x:v>-34.685275</x:v>
       </x:c>
       <x:c r="D8" s="5" t="n">
-        <x:v>30.090513</x:v>
+        <x:v>16.876437</x:v>
       </x:c>
       <x:c r="F8" s="1"/>
       <x:c r="G8" s="1"/>
@@ -768,10 +768,10 @@
         </x:is>
       </x:c>
       <x:c r="C9" s="6" t="n">
-        <x:v>-34.263653</x:v>
+        <x:v>-32.553781</x:v>
       </x:c>
       <x:c r="D9" s="5" t="n">
-        <x:v>28.524746</x:v>
+        <x:v>14.83723</x:v>
       </x:c>
       <x:c r="F9" s="1"/>
       <x:c r="G9" s="1"/>
@@ -795,10 +795,10 @@
         </x:is>
       </x:c>
       <x:c r="C10" s="6" t="n">
-        <x:v>-34.845515</x:v>
+        <x:v>-30.469595</x:v>
       </x:c>
       <x:c r="D10" s="5" t="n">
-        <x:v>26.672559</x:v>
+        <x:v>12.853821</x:v>
       </x:c>
       <x:c r="F10" s="1"/>
       <x:c r="G10" s="1"/>
@@ -822,10 +822,10 @@
         </x:is>
       </x:c>
       <x:c r="C11" s="6" t="n">
-        <x:v>-35.236355</x:v>
+        <x:v>-27.293171</x:v>
       </x:c>
       <x:c r="D11" s="5" t="n">
-        <x:v>24.53395</x:v>
+        <x:v>11.269671</x:v>
       </x:c>
       <x:c r="F11" s="1"/>
       <x:c r="G11" s="1"/>
@@ -849,10 +849,10 @@
         </x:is>
       </x:c>
       <x:c r="C12" s="6" t="n">
-        <x:v>-35.87327</x:v>
+        <x:v>-24.474346</x:v>
       </x:c>
       <x:c r="D12" s="5" t="n">
-        <x:v>21.287849</x:v>
+        <x:v>10.365769</x:v>
       </x:c>
       <x:c r="F12" s="1"/>
       <x:c r="G12" s="1"/>
@@ -876,10 +876,10 @@
         </x:is>
       </x:c>
       <x:c r="C13" s="6" t="n">
-        <x:v>-35.68738</x:v>
+        <x:v>-21.280331</x:v>
       </x:c>
       <x:c r="D13" s="5" t="n">
-        <x:v>18.710062</x:v>
+        <x:v>9.349475</x:v>
       </x:c>
       <x:c r="F13" s="1"/>
       <x:c r="G13" s="1"/>
@@ -903,10 +903,10 @@
         </x:is>
       </x:c>
       <x:c r="C14" s="6" t="n">
-        <x:v>-34.515768</x:v>
+        <x:v>-17.493437</x:v>
       </x:c>
       <x:c r="D14" s="5" t="n">
-        <x:v>16.647833</x:v>
+        <x:v>8.281086</x:v>
       </x:c>
       <x:c r="F14" s="1"/>
       <x:c r="G14" s="1"/>
@@ -930,10 +930,10 @@
         </x:is>
       </x:c>
       <x:c r="C15" s="6" t="n">
-        <x:v>-32.837986</x:v>
+        <x:v>-14.646522</x:v>
       </x:c>
       <x:c r="D15" s="5" t="n">
-        <x:v>15.349579</x:v>
+        <x:v>8.102</x:v>
       </x:c>
       <x:c r="F15" s="1"/>
       <x:c r="G15" s="1"/>

</xml_diff>